<commit_message>
rewrite all sql code to dw_ctrpn
</commit_message>
<xml_diff>
--- a/Attitude Loose/Attitude Loose/Templates/PDA Abstractor and QC Template.xlsx
+++ b/Attitude Loose/Attitude Loose/Templates/PDA Abstractor and QC Template.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="adanoa" sheetId="7" r:id="rId1"/>
-    <sheet name="gebenienee" sheetId="8" r:id="rId2"/>
-    <sheet name="otubut" sheetId="9" r:id="rId3"/>
-    <sheet name="phontharaksaj" sheetId="10" r:id="rId4"/>
+    <sheet name="Orlando Adan" sheetId="7" r:id="rId1"/>
+    <sheet name="Elena Gebeniene" sheetId="8" r:id="rId2"/>
+    <sheet name="Temisan Otubu" sheetId="9" r:id="rId3"/>
+    <sheet name="Jamie Phontharaksa" sheetId="10" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -513,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -534,40 +534,100 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="51">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -603,27 +663,73 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -650,139 +756,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -821,68 +794,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1423" displayName="Table1423" ref="A1:H3" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1423" displayName="Table1423" ref="A1:H3" totalsRowShown="0" headerRowDxfId="48" dataDxfId="18">
   <autoFilter ref="A1:H3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="49"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="48"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="47"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="46"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="45"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="44"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="43"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="42"/>
+    <tableColumn id="1" name="Trial ID" dataDxfId="26"/>
+    <tableColumn id="2" name="Submission Type" dataDxfId="25"/>
+    <tableColumn id="7" name="Submission Number" dataDxfId="24"/>
+    <tableColumn id="3" name="Abstractor" dataDxfId="23"/>
+    <tableColumn id="4" name="Abstraction Date" dataDxfId="22"/>
+    <tableColumn id="8" name="QC Date" dataDxfId="21"/>
+    <tableColumn id="5" name="Abstraction Comments" dataDxfId="20"/>
+    <tableColumn id="6" name="QC Comments" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14234" displayName="Table14234" ref="A1:H3" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14234" displayName="Table14234" ref="A1:H3" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:H3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="37"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="36"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="35"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="34"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="33"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="32"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="31"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="30"/>
+    <tableColumn id="1" name="Trial ID" dataDxfId="43"/>
+    <tableColumn id="2" name="Submission Type" dataDxfId="42"/>
+    <tableColumn id="7" name="Submission Number" dataDxfId="41"/>
+    <tableColumn id="3" name="Abstractor" dataDxfId="40"/>
+    <tableColumn id="4" name="Abstraction Date" dataDxfId="39"/>
+    <tableColumn id="8" name="QC Date" dataDxfId="38"/>
+    <tableColumn id="5" name="Abstraction Comments" dataDxfId="37"/>
+    <tableColumn id="6" name="QC Comments" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table14235" displayName="Table14235" ref="A1:H3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table14235" displayName="Table14235" ref="A1:H3" totalsRowShown="0" headerRowDxfId="33" dataDxfId="9">
   <autoFilter ref="A1:H3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="25"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="24"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="23"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="22"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="21"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="20"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="19"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="18"/>
+    <tableColumn id="1" name="Trial ID" dataDxfId="17"/>
+    <tableColumn id="2" name="Submission Type" dataDxfId="16"/>
+    <tableColumn id="7" name="Submission Number" dataDxfId="15"/>
+    <tableColumn id="3" name="Abstractor" dataDxfId="14"/>
+    <tableColumn id="4" name="Abstraction Date" dataDxfId="13"/>
+    <tableColumn id="8" name="QC Date" dataDxfId="12"/>
+    <tableColumn id="5" name="Abstraction Comments" dataDxfId="11"/>
+    <tableColumn id="6" name="QC Comments" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table14236" displayName="Table14236" ref="A1:H3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table14236" displayName="Table14236" ref="A1:H3" totalsRowShown="0" headerRowDxfId="30" dataDxfId="0">
   <autoFilter ref="A1:H3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="13"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="12"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="11"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="10"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="9"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="8"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="7"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="6"/>
+    <tableColumn id="1" name="Trial ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Submission Type" dataDxfId="7"/>
+    <tableColumn id="7" name="Submission Number" dataDxfId="6"/>
+    <tableColumn id="3" name="Abstractor" dataDxfId="5"/>
+    <tableColumn id="4" name="Abstraction Date" dataDxfId="4"/>
+    <tableColumn id="8" name="QC Date" dataDxfId="3"/>
+    <tableColumn id="5" name="Abstraction Comments" dataDxfId="2"/>
+    <tableColumn id="6" name="QC Comments" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1187,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1226,14 +1199,28 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="8"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
@@ -1933,10 +1920,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1949,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1988,14 +1975,28 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="8"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
@@ -2695,10 +2696,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="41" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2711,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2750,14 +2751,28 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="8"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
@@ -3457,10 +3472,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3473,8 +3488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3512,14 +3527,28 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="8"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
@@ -4219,10 +4248,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -9059,13 +9088,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R132:R1048576 R1">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B401">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>